<commit_message>
Agregando datros al excel
</commit_message>
<xml_diff>
--- a/LottoActivo.xlsx
+++ b/LottoActivo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaboz\Programacion\python\prediccion de numero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaboz\Programacion\python\PrediccionNumeros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7488" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7562" uniqueCount="94">
   <si>
     <t>Fecha</t>
   </si>
@@ -197,13 +197,119 @@
   <si>
     <t>12:00</t>
   </si>
+  <si>
+    <t>Pescado</t>
+  </si>
+  <si>
+    <t>Toro</t>
+  </si>
+  <si>
+    <t>Cebra</t>
+  </si>
+  <si>
+    <t>Mono</t>
+  </si>
+  <si>
+    <t>Zorro</t>
+  </si>
+  <si>
+    <t>Cochino</t>
+  </si>
+  <si>
+    <t>Culebra</t>
+  </si>
+  <si>
+    <t>Ballena</t>
+  </si>
+  <si>
+    <t>Ardilla</t>
+  </si>
+  <si>
+    <t>Caballo</t>
+  </si>
+  <si>
+    <t>Gato</t>
+  </si>
+  <si>
+    <t>Zamuro</t>
+  </si>
+  <si>
+    <t>Oso</t>
+  </si>
+  <si>
+    <t>Elefante</t>
+  </si>
+  <si>
+    <t>Gallo</t>
+  </si>
+  <si>
+    <t>Aguila</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>Gallina</t>
+  </si>
+  <si>
+    <t>Raton</t>
+  </si>
+  <si>
+    <t>Chivo</t>
+  </si>
+  <si>
+    <t>Iguana</t>
+  </si>
+  <si>
+    <t>Perro</t>
+  </si>
+  <si>
+    <t>Ciempies</t>
+  </si>
+  <si>
+    <t>Perico</t>
+  </si>
+  <si>
+    <t>Jirafa</t>
+  </si>
+  <si>
+    <t>Venado</t>
+  </si>
+  <si>
+    <t>Tigre</t>
+  </si>
+  <si>
+    <t>Delfin</t>
+  </si>
+  <si>
+    <t>Rana</t>
+  </si>
+  <si>
+    <t>Burro</t>
+  </si>
+  <si>
+    <t>Paloma</t>
+  </si>
+  <si>
+    <t>Vaca</t>
+  </si>
+  <si>
+    <t>Lapa</t>
+  </si>
+  <si>
+    <t>Alacran</t>
+  </si>
+  <si>
+    <t>Camello</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="170" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -254,12 +360,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,13 +671,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3743"/>
+  <dimension ref="A1:D3817"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3711" workbookViewId="0">
-      <selection activeCell="C3743" sqref="C3743"/>
+    <sheetView tabSelected="1" topLeftCell="A3740" workbookViewId="0">
+      <selection activeCell="D3758" sqref="D3758"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -52682,297 +52794,1154 @@
       <c r="A3723" s="2">
         <v>45989</v>
       </c>
-      <c r="B3723" t="s">
-        <v>19</v>
+      <c r="B3723" s="3">
+        <v>0.375</v>
       </c>
       <c r="C3723" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D3723">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3724" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3724" s="2">
         <v>45989</v>
       </c>
-      <c r="B3724" t="s">
-        <v>21</v>
+      <c r="B3724" s="3">
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3724" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D3724">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3725" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3725" s="2">
         <v>45989</v>
       </c>
-      <c r="B3725" t="s">
-        <v>23</v>
+      <c r="B3725" s="3">
+        <v>0.45833333333333331</v>
       </c>
       <c r="C3725" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D3725">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3726" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3726" s="2">
         <v>45989</v>
       </c>
-      <c r="B3726" t="s">
-        <v>25</v>
+      <c r="B3726" s="3">
+        <v>0.5</v>
       </c>
       <c r="C3726" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D3726">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3727" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3727" s="2">
-        <v>45990</v>
-      </c>
-      <c r="B3727" t="s">
-        <v>4</v>
+        <v>45989</v>
+      </c>
+      <c r="B3727" s="3">
+        <v>0.54166666666666663</v>
       </c>
       <c r="C3727" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D3727">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3728" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3728" s="2">
-        <v>45990</v>
-      </c>
-      <c r="B3728" t="s">
-        <v>6</v>
+        <v>45989</v>
+      </c>
+      <c r="B3728" s="3">
+        <v>0.58333333333333337</v>
       </c>
       <c r="C3728" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D3728">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3729" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3729" s="2">
-        <v>45990</v>
-      </c>
-      <c r="B3729" t="s">
-        <v>8</v>
+        <v>45989</v>
+      </c>
+      <c r="B3729" s="3">
+        <v>0.625</v>
       </c>
       <c r="C3729" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D3729">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3730" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3730" s="2">
-        <v>45990</v>
-      </c>
-      <c r="B3730" t="s">
-        <v>10</v>
+        <v>45989</v>
+      </c>
+      <c r="B3730" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C3730" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D3730">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3731" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3731" s="2">
-        <v>45990</v>
-      </c>
-      <c r="B3731" t="s">
-        <v>12</v>
+        <v>45989</v>
+      </c>
+      <c r="B3731" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C3731" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D3731">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3732" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3732" s="2">
-        <v>45990</v>
-      </c>
-      <c r="B3732" t="s">
-        <v>14</v>
+        <v>45989</v>
+      </c>
+      <c r="B3732" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C3732" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D3732">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3733" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3733" s="2">
-        <v>45990</v>
-      </c>
-      <c r="B3733" t="s">
+        <v>45989</v>
+      </c>
+      <c r="B3733" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3733" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3733">
         <v>16</v>
-      </c>
-      <c r="C3733" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3733">
-        <v>11</v>
       </c>
     </row>
     <row r="3734" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3734" s="2">
         <v>45990</v>
       </c>
-      <c r="B3734" t="s">
-        <v>18</v>
+      <c r="B3734" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C3734" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D3734">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3735" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3735" s="2">
         <v>45990</v>
       </c>
-      <c r="B3735" t="s">
-        <v>19</v>
+      <c r="B3735" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C3735" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D3735">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3736" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3736" s="2">
         <v>45990</v>
       </c>
-      <c r="B3736" t="s">
-        <v>21</v>
+      <c r="B3736" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C3736" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D3736">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3737" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3737" s="2">
         <v>45990</v>
       </c>
-      <c r="B3737" t="s">
-        <v>23</v>
+      <c r="B3737" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C3737" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D3737">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3738" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3738" s="2">
         <v>45990</v>
       </c>
-      <c r="B3738" t="s">
-        <v>25</v>
+      <c r="B3738" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C3738" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D3738">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3739" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3739" s="2">
-        <v>45991</v>
-      </c>
-      <c r="B3739" t="s">
-        <v>54</v>
+        <v>45990</v>
+      </c>
+      <c r="B3739" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C3739" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D3739">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3740" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3740" s="2">
-        <v>45991</v>
-      </c>
-      <c r="B3740" t="s">
-        <v>55</v>
+        <v>45990</v>
+      </c>
+      <c r="B3740" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C3740" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D3740">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3741" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3741" s="2">
-        <v>45991</v>
-      </c>
-      <c r="B3741" t="s">
-        <v>56</v>
+        <v>45990</v>
+      </c>
+      <c r="B3741" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C3741" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3741">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3742" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3742" s="2">
-        <v>45991</v>
-      </c>
-      <c r="B3742" t="s">
-        <v>57</v>
+        <v>45990</v>
+      </c>
+      <c r="B3742" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C3742" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="D3742">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3743" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3743" s="2">
+        <v>45990</v>
+      </c>
+      <c r="B3743" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3743" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3743">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3744" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3744" s="2">
+        <v>45990</v>
+      </c>
+      <c r="B3744" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3744" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3744">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3745" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3745" s="2">
+        <v>45990</v>
+      </c>
+      <c r="B3745" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3745" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3745">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3746" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3746" s="2">
         <v>45991</v>
       </c>
-      <c r="B3743" t="s">
+      <c r="B3746" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3746" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3746">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3747" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3747" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3747" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3747" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3747">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3748" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3748" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3748" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3748" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3748">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3749" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3749" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3749" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3749" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3749">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3750" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3750" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3750" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C3743" t="s">
+      <c r="C3750" t="s">
         <v>28</v>
       </c>
-      <c r="D3743">
+      <c r="D3750">
         <v>37</v>
+      </c>
+    </row>
+    <row r="3751" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3751" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3751" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3751" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3751">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3752" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3752" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3752" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C3752" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3752">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3753" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3753" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3753" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C3753" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3753">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3754" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3754" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3754" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3754" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3754">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3755" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3755" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3755" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C3755" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3755">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3756" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3756" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3756" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C3756" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3756">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3757" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3757" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B3757" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C3757" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3757">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3758" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3758" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3758" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3758" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3759" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3759" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3759" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C3759" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3760" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3760" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3760" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3760" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3761" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3761" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3761" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C3761" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3762" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3762" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3762" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3762" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3763" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3763" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3763" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3763" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3764" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3764" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3764" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C3764" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3765" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3765" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3765" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C3765" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3766" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3766" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3766" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3766" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3767" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3767" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3767" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C3767" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3768" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3768" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3768" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C3768" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3769" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3769" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B3769" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C3769" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3770" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3770" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3770" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3770" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3771" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3771" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3771" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C3771" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3772" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3772" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3772" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3772" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3773" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3773" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3773" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C3773" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3774" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3774" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3774" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3774" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3775" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3775" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3775" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3775" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3776" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3776" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3776" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C3776" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3777" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3777" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3777" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C3777" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3778" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3778" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3778" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3778" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3779" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3779" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3779" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C3779" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3780" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3780" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3780" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C3780" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3781" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3781" s="2">
+        <v>45993</v>
+      </c>
+      <c r="B3781" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C3781" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3782" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3782" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3782" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3782" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3783" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3783" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3783" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C3783" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3784" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3784" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3784" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3784" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3785" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3785" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3785" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C3785" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3786" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3786" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3786" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3786" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3787" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3787" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3787" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3787" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3788" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3788" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3788" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C3788" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3789" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3789" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3789" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C3789" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3790" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3790" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3790" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3790" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3791" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3791" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3791" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C3791" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3792" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3792" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3792" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C3792" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3793" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3793" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B3793" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C3793" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3794" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3794" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3794" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3794" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3795" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3795" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3795" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C3795" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3796" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3796" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3796" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3796" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3797" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3797" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3797" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C3797" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3798" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3798" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3798" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3798" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3799" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3799" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3799" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3799" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3800" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3800" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3800" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C3800" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3801" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3801" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3801" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C3801" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3802" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3802" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3802" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3802" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3803" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3803" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3803" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C3803" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3804" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3804" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3804" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C3804" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3805" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3805" s="2">
+        <v>45995</v>
+      </c>
+      <c r="B3805" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C3805" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3806" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3806" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3806" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3806" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3807" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3807" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3807" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C3807" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3808" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3808" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3808" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3808" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3809" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3809" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3809" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C3809" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3810" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3810" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3810" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3810" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3811" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3811" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3811" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3811" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3812" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3812" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3812" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C3812" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3813" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3813" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3813" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C3813" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3814" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3814" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3814" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3814" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3815" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3815" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3815" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C3815" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3816" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3816" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C3816" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3817" s="2">
+        <v>45996</v>
+      </c>
+      <c r="B3817" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C3817" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>